<commit_message>
Updated notebook analysis and output
</commit_message>
<xml_diff>
--- a/recommended_trades.xlsx
+++ b/recommended_trades.xlsx
@@ -4562,10 +4562,10 @@
         <v>192</v>
       </c>
       <c r="B190" s="2">
-        <v>305.8</v>
+        <v>303.26</v>
       </c>
       <c r="C190" s="2">
-        <v>22078760000</v>
+        <v>21895372000</v>
       </c>
       <c r="D190" s="3">
         <v>6</v>

</xml_diff>